<commit_message>
fix SRS requirements numbering
</commit_message>
<xml_diff>
--- a/Requirements_Specification/SafePath_SRS.xlsx
+++ b/Requirements_Specification/SafePath_SRS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/huda.khalil/Documents/TeamProject/SRS-Doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35B2F390-78C4-134D-8D1A-C273450FEC04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E92261EA-D93A-D34C-9DC7-B2FA2F5C5964}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="980" windowWidth="27040" windowHeight="16380" xr2:uid="{43BAFF81-32F0-934D-BBDE-E19BC4484916}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="59">
   <si>
     <t>Requirement Specification</t>
   </si>
@@ -222,6 +222,9 @@
   </si>
   <si>
     <t>add login/signup pages</t>
+  </si>
+  <si>
+    <t>R12</t>
   </si>
 </sst>
 </file>
@@ -322,27 +325,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="14">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -393,14 +381,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </left>
-      <right/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -414,6 +404,21 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -424,28 +429,28 @@
         <color indexed="64"/>
       </left>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -454,38 +459,40 @@
         <color indexed="64"/>
       </left>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </top>
       <bottom style="medium">
         <color indexed="64"/>
@@ -494,144 +501,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </left>
-      <right/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </top>
       <bottom style="medium">
         <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
@@ -639,124 +518,100 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1079,8 +934,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F71F488F-97B4-7E4A-9F02-176F07B043AA}">
   <dimension ref="B1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="81" zoomScaleNormal="81" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1093,316 +948,316 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:10" ht="62" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
     </row>
     <row r="2" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:10" ht="20" x14ac:dyDescent="0.2">
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="G3" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="17" t="s">
+      <c r="H3" s="7" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="4" spans="2:10" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="D4" s="23" t="s">
+      <c r="D4" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="E4" s="23" t="s">
+      <c r="E4" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="24" t="s">
+      <c r="F4" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="25" t="s">
+      <c r="G4" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="H4" s="26"/>
+      <c r="H4" s="22"/>
       <c r="J4" s="1"/>
     </row>
     <row r="5" spans="2:10" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="36" t="s">
+      <c r="C5" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="D5" s="27" t="s">
+      <c r="D5" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="E5" s="27" t="s">
+      <c r="E5" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="28" t="s">
+      <c r="F5" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="29" t="s">
+      <c r="G5" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="H5" s="30"/>
+      <c r="H5" s="24"/>
       <c r="J5" s="1"/>
     </row>
     <row r="6" spans="2:10" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="35"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="27" t="s">
+      <c r="B6" s="23"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="E6" s="27" t="s">
+      <c r="E6" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="28" t="s">
+      <c r="F6" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="29" t="s">
+      <c r="G6" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="H6" s="30"/>
+      <c r="H6" s="24"/>
       <c r="J6" s="1"/>
     </row>
     <row r="7" spans="2:10" ht="40" x14ac:dyDescent="0.2">
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="F7" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G7" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="H7" s="11"/>
+      <c r="H7" s="26"/>
     </row>
     <row r="8" spans="2:10" ht="60" x14ac:dyDescent="0.2">
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="F8" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="10" t="s">
+      <c r="G8" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="H8" s="11"/>
+      <c r="H8" s="26"/>
       <c r="J8" s="1"/>
     </row>
     <row r="9" spans="2:10" ht="60" x14ac:dyDescent="0.2">
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="F9" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="G9" s="10" t="s">
+      <c r="G9" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="H9" s="11"/>
+      <c r="H9" s="26"/>
       <c r="I9" s="1"/>
     </row>
     <row r="10" spans="2:10" ht="60" x14ac:dyDescent="0.2">
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E10" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="F10" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="10" t="s">
+      <c r="G10" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="H10" s="11"/>
+      <c r="H10" s="26"/>
       <c r="J10" s="1"/>
     </row>
     <row r="11" spans="2:10" ht="40" x14ac:dyDescent="0.2">
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="F11" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="G11" s="10" t="s">
+      <c r="G11" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="H11" s="11"/>
+      <c r="H11" s="26"/>
       <c r="J11" s="1"/>
     </row>
     <row r="12" spans="2:10" ht="40" x14ac:dyDescent="0.2">
-      <c r="B12" s="39" t="s">
+      <c r="B12" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="E12" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F12" s="9" t="s">
+      <c r="F12" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="10" t="s">
+      <c r="G12" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="H12" s="11"/>
+      <c r="H12" s="26"/>
       <c r="J12" s="1"/>
     </row>
     <row r="13" spans="2:10" ht="80" x14ac:dyDescent="0.2">
-      <c r="B13" s="38" t="s">
-        <v>46</v>
-      </c>
-      <c r="C13" s="18" t="s">
+      <c r="B13" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="18" t="s">
+      <c r="D13" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="18" t="s">
+      <c r="E13" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F13" s="19" t="s">
+      <c r="F13" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="G13" s="20" t="s">
+      <c r="G13" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="H13" s="21"/>
+      <c r="H13" s="28"/>
     </row>
     <row r="14" spans="2:10" ht="60" x14ac:dyDescent="0.2">
-      <c r="B14" s="38" t="s">
-        <v>51</v>
-      </c>
-      <c r="C14" s="18" t="s">
+      <c r="B14" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="18" t="s">
+      <c r="D14" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E14" s="18" t="s">
+      <c r="E14" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F14" s="19" t="s">
+      <c r="F14" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="G14" s="20" t="s">
+      <c r="G14" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="H14" s="21"/>
+      <c r="H14" s="28"/>
     </row>
     <row r="15" spans="2:10" ht="40" x14ac:dyDescent="0.2">
-      <c r="B15" s="38" t="s">
-        <v>52</v>
-      </c>
-      <c r="C15" s="18" t="s">
+      <c r="B15" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="18" t="s">
+      <c r="D15" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E15" s="18" t="s">
+      <c r="E15" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F15" s="19" t="s">
+      <c r="F15" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="G15" s="20" t="s">
+      <c r="G15" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="H15" s="21"/>
+      <c r="H15" s="28"/>
     </row>
     <row r="16" spans="2:10" ht="61" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="C16" s="12" t="s">
+      <c r="B16" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E16" s="12" t="s">
+      <c r="E16" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F16" s="13" t="s">
+      <c r="F16" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="G16" s="14" t="s">
+      <c r="G16" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="H16" s="15"/>
+      <c r="H16" s="31"/>
     </row>
     <row r="17" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>
@@ -1414,10 +1269,10 @@
       <c r="H17" s="1"/>
     </row>
     <row r="18" spans="2:8" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="32" t="s">
+      <c r="B18" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="33"/>
+      <c r="C18" s="13"/>
       <c r="D18" s="4" t="s">
         <v>35</v>
       </c>

</xml_diff>

<commit_message>
update SRS document according to project progress
</commit_message>
<xml_diff>
--- a/Requirements_Specification/SafePath_SRS.xlsx
+++ b/Requirements_Specification/SafePath_SRS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/huda.khalil/Documents/TeamProject/SRS-Doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E92261EA-D93A-D34C-9DC7-B2FA2F5C5964}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{452D8B05-D7EC-9C4C-9DAD-456FFA1DABE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="980" windowWidth="27040" windowHeight="16380" xr2:uid="{43BAFF81-32F0-934D-BBDE-E19BC4484916}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="62">
   <si>
     <t>Requirement Specification</t>
   </si>
@@ -126,9 +126,6 @@
   </si>
   <si>
     <t>Week 7</t>
-  </si>
-  <si>
-    <t>Week 8</t>
   </si>
   <si>
     <t>from week 3 till the end</t>
@@ -225,6 +222,18 @@
   </si>
   <si>
     <t>R12</t>
+  </si>
+  <si>
+    <t>Week 9</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>Status</t>
   </si>
 </sst>
 </file>
@@ -293,7 +302,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -312,20 +321,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCED7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="14">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -514,11 +511,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -544,10 +580,34 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -559,59 +619,39 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -932,10 +972,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F71F488F-97B4-7E4A-9F02-176F07B043AA}">
-  <dimension ref="B1:J21"/>
+  <dimension ref="B1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="81" zoomScaleNormal="81" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="135" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -943,244 +983,269 @@
     <col min="1" max="1" width="2" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
     <col min="4" max="4" width="42" customWidth="1"/>
-    <col min="6" max="7" width="18.5" customWidth="1"/>
-    <col min="8" max="8" width="22.83203125" customWidth="1"/>
+    <col min="6" max="8" width="18.5" customWidth="1"/>
+    <col min="9" max="9" width="22.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="62" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B1" s="11" t="s">
+    <row r="1" spans="2:11" ht="62" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-    </row>
-    <row r="2" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="2:10" ht="20" x14ac:dyDescent="0.2">
-      <c r="B3" s="19" t="s">
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+    </row>
+    <row r="2" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="2:11" ht="20" x14ac:dyDescent="0.2">
+      <c r="B3" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="20" t="s">
+      <c r="E3" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="20" t="s">
+      <c r="F3" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="20" t="s">
+      <c r="G3" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="H4" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="I4" s="25"/>
+      <c r="K4" s="1"/>
+    </row>
+    <row r="5" spans="2:11" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="33" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="I5" s="25"/>
+      <c r="K5" s="1"/>
+    </row>
+    <row r="6" spans="2:11" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="32"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="I6" s="25"/>
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7" spans="2:11" s="26" customFormat="1" ht="40" x14ac:dyDescent="0.2">
+      <c r="B7" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="23" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="4" spans="2:10" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="E4" s="9" t="s">
+      <c r="E7" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F7" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="H4" s="22"/>
-      <c r="J4" s="1"/>
-    </row>
-    <row r="5" spans="2:10" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="E5" s="10" t="s">
+      <c r="G7" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="H7" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="I7" s="25"/>
+    </row>
+    <row r="8" spans="2:11" s="26" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+      <c r="B8" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="H5" s="24"/>
-      <c r="J5" s="1"/>
-    </row>
-    <row r="6" spans="2:10" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="23"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="G6" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="H6" s="24"/>
-      <c r="J6" s="1"/>
-    </row>
-    <row r="7" spans="2:10" ht="40" x14ac:dyDescent="0.2">
-      <c r="B7" s="25" t="s">
-        <v>41</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="H7" s="26"/>
-    </row>
-    <row r="8" spans="2:10" ht="60" x14ac:dyDescent="0.2">
-      <c r="B8" s="25" t="s">
+      <c r="F8" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="H8" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="I8" s="25"/>
+    </row>
+    <row r="9" spans="2:11" s="26" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+      <c r="B9" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H8" s="26"/>
-      <c r="J8" s="1"/>
-    </row>
-    <row r="9" spans="2:10" ht="60" x14ac:dyDescent="0.2">
-      <c r="B9" s="25" t="s">
-        <v>43</v>
-      </c>
       <c r="C9" s="5" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="17" t="s">
+      <c r="F9" s="9" t="s">
         <v>14</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="H9" s="26"/>
-      <c r="I9" s="1"/>
-    </row>
-    <row r="10" spans="2:10" ht="60" x14ac:dyDescent="0.2">
-      <c r="B10" s="25" t="s">
+      <c r="H9" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="I9" s="13"/>
+    </row>
+    <row r="10" spans="2:11" ht="60" x14ac:dyDescent="0.2">
+      <c r="B10" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H10" s="29"/>
+      <c r="I10" s="13"/>
+      <c r="K10" s="1"/>
+    </row>
+    <row r="11" spans="2:11" ht="40" x14ac:dyDescent="0.2">
+      <c r="B11" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F10" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H10" s="26"/>
-      <c r="J10" s="1"/>
-    </row>
-    <row r="11" spans="2:10" ht="40" x14ac:dyDescent="0.2">
-      <c r="B11" s="25" t="s">
-        <v>45</v>
-      </c>
       <c r="C11" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>54</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>55</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F11" s="17" t="s">
+      <c r="F11" s="9" t="s">
         <v>9</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="H11" s="26"/>
-      <c r="J11" s="1"/>
-    </row>
-    <row r="12" spans="2:10" ht="40" x14ac:dyDescent="0.2">
-      <c r="B12" s="25" t="s">
-        <v>46</v>
+        <v>58</v>
+      </c>
+      <c r="H11" s="29"/>
+      <c r="I11" s="13"/>
+      <c r="K11" s="1"/>
+    </row>
+    <row r="12" spans="2:11" ht="40" x14ac:dyDescent="0.2">
+      <c r="B12" s="22" t="s">
+        <v>45</v>
       </c>
       <c r="C12" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>56</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>57</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F12" s="17" t="s">
+      <c r="F12" s="9" t="s">
         <v>9</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="H12" s="26"/>
-      <c r="J12" s="1"/>
-    </row>
-    <row r="13" spans="2:10" ht="80" x14ac:dyDescent="0.2">
-      <c r="B13" s="27" t="s">
-        <v>51</v>
+      <c r="H12" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="I12" s="13"/>
+      <c r="K12" s="1"/>
+    </row>
+    <row r="13" spans="2:11" ht="80" x14ac:dyDescent="0.2">
+      <c r="B13" s="14" t="s">
+        <v>50</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D13" s="8" t="s">
         <v>17</v>
@@ -1188,17 +1253,18 @@
       <c r="E13" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F13" s="18" t="s">
+      <c r="F13" s="10" t="s">
         <v>19</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="H13" s="28"/>
-    </row>
-    <row r="14" spans="2:10" ht="60" x14ac:dyDescent="0.2">
-      <c r="B14" s="27" t="s">
-        <v>52</v>
+        <v>35</v>
+      </c>
+      <c r="H13" s="30"/>
+      <c r="I13" s="15"/>
+    </row>
+    <row r="14" spans="2:11" ht="60" x14ac:dyDescent="0.2">
+      <c r="B14" s="14" t="s">
+        <v>51</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>22</v>
@@ -1209,17 +1275,18 @@
       <c r="E14" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F14" s="18" t="s">
+      <c r="F14" s="10" t="s">
         <v>14</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="H14" s="28"/>
-    </row>
-    <row r="15" spans="2:10" ht="40" x14ac:dyDescent="0.2">
-      <c r="B15" s="27" t="s">
-        <v>53</v>
+        <v>35</v>
+      </c>
+      <c r="H14" s="30"/>
+      <c r="I14" s="15"/>
+    </row>
+    <row r="15" spans="2:11" ht="40" x14ac:dyDescent="0.2">
+      <c r="B15" s="14" t="s">
+        <v>52</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>24</v>
@@ -1230,17 +1297,18 @@
       <c r="E15" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F15" s="18" t="s">
+      <c r="F15" s="10" t="s">
         <v>9</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="H15" s="28"/>
-    </row>
-    <row r="16" spans="2:10" ht="61" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="29" t="s">
-        <v>58</v>
+        <v>35</v>
+      </c>
+      <c r="H15" s="30"/>
+      <c r="I15" s="15"/>
+    </row>
+    <row r="16" spans="2:11" ht="61" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="16" t="s">
+        <v>57</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>26</v>
@@ -1251,38 +1319,42 @@
       <c r="E16" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F16" s="30" t="s">
+      <c r="F16" s="17" t="s">
         <v>9</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="H16" s="31"/>
-    </row>
-    <row r="17" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="H16" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="I16" s="18"/>
+    </row>
+    <row r="17" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
-      <c r="H17" s="1"/>
-    </row>
-    <row r="18" spans="2:8" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="12" t="s">
+      <c r="H17" s="3"/>
+      <c r="I17" s="1"/>
+    </row>
+    <row r="18" spans="2:9" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="21"/>
+      <c r="D18" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="13"/>
-      <c r="D18" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8" ht="40" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="20" spans="2:8" ht="40" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="21" spans="2:8" ht="40" customHeight="1" x14ac:dyDescent="0.2"/>
+    </row>
+    <row r="19" spans="2:9" ht="40" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" spans="2:9" ht="40" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="21" spans="2:9" ht="40" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B1:I1"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="C5:C6"/>

</xml_diff>

<commit_message>
Adding SRS updates after Andrea follow up meeting
</commit_message>
<xml_diff>
--- a/Requirements_Specification/SafePath_SRS.xlsx
+++ b/Requirements_Specification/SafePath_SRS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/huda.khalil/Documents/TeamProject/SRS-Doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{452D8B05-D7EC-9C4C-9DAD-456FFA1DABE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B708ED5-50F8-104E-ACF0-E66BA5C7F902}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="980" windowWidth="27040" windowHeight="16380" xr2:uid="{43BAFF81-32F0-934D-BBDE-E19BC4484916}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="66">
   <si>
     <t>Requirement Specification</t>
   </si>
@@ -74,12 +74,6 @@
     <t>score routes</t>
   </si>
   <si>
-    <t>score routes using real safety factors (crime, lighting, crashes, hazards, traffic) so user feel more confident journey.</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
     <t>All cyclists/ Pedestrians/ city planners</t>
   </si>
   <si>
@@ -134,10 +128,103 @@
     <t xml:space="preserve">display secure bike parking </t>
   </si>
   <si>
-    <t>Release 1.0/Week 5</t>
-  </si>
-  <si>
     <t>Non-Functional Requirments:</t>
+  </si>
+  <si>
+    <t>Futur work</t>
+  </si>
+  <si>
+    <t>suggest multiple routes (fastest, safest)</t>
+  </si>
+  <si>
+    <t>R02</t>
+  </si>
+  <si>
+    <t>search route</t>
+  </si>
+  <si>
+    <t>R04</t>
+  </si>
+  <si>
+    <t>R05</t>
+  </si>
+  <si>
+    <t>R06</t>
+  </si>
+  <si>
+    <t>R07</t>
+  </si>
+  <si>
+    <t>R08</t>
+  </si>
+  <si>
+    <t>search fastest route</t>
+  </si>
+  <si>
+    <t>search for fastest route, speed factor only</t>
+  </si>
+  <si>
+    <t>R09</t>
+  </si>
+  <si>
+    <t>R10</t>
+  </si>
+  <si>
+    <t>R11</t>
+  </si>
+  <si>
+    <t>find cycle/walk buddy</t>
+  </si>
+  <si>
+    <t>find cycle/ walker buddy to share ride with nearby</t>
+  </si>
+  <si>
+    <t>save user credentials</t>
+  </si>
+  <si>
+    <t>add login/signup pages</t>
+  </si>
+  <si>
+    <t>R12</t>
+  </si>
+  <si>
+    <t>Week 9</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Shalini</t>
+  </si>
+  <si>
+    <t>Priyanka &amp; Karan</t>
+  </si>
+  <si>
+    <t>Owner</t>
+  </si>
+  <si>
+    <t>Huda</t>
+  </si>
+  <si>
+    <t>Add customizable safety factors to the profile page (crime, lighting, crashes, hazards, traffic) so each user can set their own safety preferences for route suggestions.</t>
+  </si>
+  <si>
+    <t>Week 5</t>
+  </si>
+  <si>
+    <t>Week 8</t>
+  </si>
+  <si>
+    <t>search for safest route according to safety factors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shalini &amp; </t>
   </si>
   <si>
     <r>
@@ -145,102 +232,26 @@
     </r>
     <r>
       <rPr>
-        <sz val="12"/>
+        <sz val="14"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
-        <scheme val="minor"/>
       </rPr>
       <t>want personal data handled securely and in line with GDPR.</t>
     </r>
   </si>
   <si>
-    <t>Futur work</t>
-  </si>
-  <si>
-    <t>Technology</t>
-  </si>
-  <si>
-    <t>suggest multiple routes (fastest, safest)</t>
-  </si>
-  <si>
-    <t>R02</t>
-  </si>
-  <si>
-    <t>search route</t>
-  </si>
-  <si>
-    <t>R03</t>
-  </si>
-  <si>
-    <t>R04</t>
-  </si>
-  <si>
-    <t>R05</t>
-  </si>
-  <si>
-    <t>R06</t>
-  </si>
-  <si>
-    <t>R07</t>
-  </si>
-  <si>
-    <t>R08</t>
-  </si>
-  <si>
-    <t>search fastest route</t>
-  </si>
-  <si>
-    <t>search for fastest route, speed factor only</t>
-  </si>
-  <si>
-    <t xml:space="preserve">search for safest route, safety - crim factor </t>
-  </si>
-  <si>
-    <t xml:space="preserve">search for safest route, safety - hazard factor  </t>
-  </si>
-  <si>
-    <t>R09</t>
-  </si>
-  <si>
-    <t>R10</t>
-  </si>
-  <si>
-    <t>R11</t>
-  </si>
-  <si>
-    <t>find cycle/walk buddy</t>
-  </si>
-  <si>
-    <t>find cycle/ walker buddy to share ride with nearby</t>
-  </si>
-  <si>
-    <t>save user credentials</t>
-  </si>
-  <si>
-    <t>add login/signup pages</t>
-  </si>
-  <si>
-    <t>R12</t>
-  </si>
-  <si>
-    <t>Week 9</t>
-  </si>
-  <si>
-    <t>Done</t>
-  </si>
-  <si>
-    <t>In Progress</t>
-  </si>
-  <si>
-    <t>Status</t>
+    <t>Priyanka &amp; Huda</t>
+  </si>
+  <si>
+    <t>All Team</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -275,15 +286,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -292,17 +294,38 @@
     <font>
       <sz val="14"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -321,8 +344,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCED7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="17">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -550,11 +579,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -565,93 +620,111 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -972,35 +1045,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F71F488F-97B4-7E4A-9F02-176F07B043AA}">
-  <dimension ref="B1:K21"/>
+  <dimension ref="B1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="135" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="84" zoomScaleNormal="135" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="4" width="42" customWidth="1"/>
-    <col min="6" max="8" width="18.5" customWidth="1"/>
-    <col min="9" max="9" width="22.83203125" customWidth="1"/>
+    <col min="4" max="4" width="71.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="6" max="6" width="38.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.83203125" style="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="62" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
     </row>
     <row r="2" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="2:11" ht="20" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:11" s="15" customFormat="1" ht="52" x14ac:dyDescent="0.2">
       <c r="B3" s="11" t="s">
         <v>1</v>
       </c>
@@ -1019,345 +1096,337 @@
       <c r="G3" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="27" t="s">
+      <c r="H3" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" ht="20" x14ac:dyDescent="0.2">
+      <c r="B4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="I4" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="K4" s="1"/>
+    </row>
+    <row r="5" spans="2:11" s="18" customFormat="1" ht="20" x14ac:dyDescent="0.2">
+      <c r="B5" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="I3" s="7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="2:11" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="D4" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="E4" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="H4" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="I4" s="25"/>
-      <c r="K4" s="1"/>
-    </row>
-    <row r="5" spans="2:11" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="32" t="s">
-        <v>38</v>
-      </c>
-      <c r="C5" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="E5" s="23" t="s">
+      <c r="E5" s="22" t="s">
         <v>8</v>
       </c>
       <c r="F5" s="24" t="s">
         <v>9</v>
       </c>
       <c r="G5" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="H5" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="I5" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="K5" s="19"/>
+    </row>
+    <row r="6" spans="2:11" s="18" customFormat="1" ht="38" x14ac:dyDescent="0.2">
+      <c r="B6" s="27"/>
+      <c r="C6" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="H5" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="I5" s="25"/>
-      <c r="K5" s="1"/>
-    </row>
-    <row r="6" spans="2:11" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="32"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="23" t="s">
-        <v>49</v>
-      </c>
-      <c r="E6" s="23" t="s">
+      <c r="E6" s="22" t="s">
         <v>8</v>
       </c>
       <c r="F6" s="24" t="s">
         <v>9</v>
       </c>
       <c r="G6" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="H6" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="I6" s="25"/>
-      <c r="K6" s="1"/>
-    </row>
-    <row r="7" spans="2:11" s="26" customFormat="1" ht="40" x14ac:dyDescent="0.2">
-      <c r="B7" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="C7" s="23" t="s">
-        <v>10</v>
+      <c r="H6" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="I6" s="26" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" ht="38" x14ac:dyDescent="0.2">
+      <c r="B7" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>13</v>
       </c>
       <c r="D7" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="I7" s="26" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" ht="38" x14ac:dyDescent="0.2">
+      <c r="B8" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="H8" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="I8" s="26" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" ht="57" x14ac:dyDescent="0.2">
+      <c r="B9" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="E7" s="23" t="s">
+      <c r="C9" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="24" t="s">
+      <c r="F9" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="H9" s="25"/>
+      <c r="I9" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="K9" s="1"/>
+    </row>
+    <row r="10" spans="2:11" ht="19" x14ac:dyDescent="0.2">
+      <c r="B10" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="23" t="s">
+      <c r="G10" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="H10" s="9"/>
+      <c r="I10" s="20"/>
+      <c r="K10" s="1"/>
+    </row>
+    <row r="11" spans="2:11" ht="20" x14ac:dyDescent="0.2">
+      <c r="B11" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="I11" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="K11" s="1"/>
+    </row>
+    <row r="12" spans="2:11" ht="57" x14ac:dyDescent="0.2">
+      <c r="B12" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="H7" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="I7" s="25"/>
-    </row>
-    <row r="8" spans="2:11" s="26" customFormat="1" ht="60" x14ac:dyDescent="0.2">
-      <c r="B8" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="C8" s="23" t="s">
+      <c r="D12" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="23" t="s">
+      <c r="E12" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="23" t="s">
+      <c r="F12" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="H12" s="4"/>
+      <c r="I12" s="16"/>
+    </row>
+    <row r="13" spans="2:11" ht="38" x14ac:dyDescent="0.2">
+      <c r="B13" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="H13" s="4"/>
+      <c r="I13" s="16"/>
+    </row>
+    <row r="14" spans="2:11" ht="38" x14ac:dyDescent="0.2">
+      <c r="B14" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="H14" s="4"/>
+      <c r="I14" s="16"/>
+    </row>
+    <row r="15" spans="2:11" ht="38" x14ac:dyDescent="0.2">
+      <c r="B15" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="G8" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="H8" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="I8" s="25"/>
-    </row>
-    <row r="9" spans="2:11" s="26" customFormat="1" ht="60" x14ac:dyDescent="0.2">
-      <c r="B9" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H9" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="I9" s="13"/>
-    </row>
-    <row r="10" spans="2:11" ht="60" x14ac:dyDescent="0.2">
-      <c r="B10" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="H10" s="29"/>
-      <c r="I10" s="13"/>
-      <c r="K10" s="1"/>
-    </row>
-    <row r="11" spans="2:11" ht="40" x14ac:dyDescent="0.2">
-      <c r="B11" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F11" s="9" t="s">
+      <c r="F15" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="G11" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="H11" s="29"/>
-      <c r="I11" s="13"/>
-      <c r="K11" s="1"/>
-    </row>
-    <row r="12" spans="2:11" ht="40" x14ac:dyDescent="0.2">
-      <c r="B12" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F12" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="G12" s="5" t="s">
+      <c r="G15" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="H12" s="29" t="s">
-        <v>59</v>
-      </c>
-      <c r="I12" s="13"/>
-      <c r="K12" s="1"/>
-    </row>
-    <row r="13" spans="2:11" ht="80" x14ac:dyDescent="0.2">
-      <c r="B13" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="G13" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="H13" s="30"/>
-      <c r="I13" s="15"/>
-    </row>
-    <row r="14" spans="2:11" ht="60" x14ac:dyDescent="0.2">
-      <c r="B14" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="F14" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="G14" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="H14" s="30"/>
-      <c r="I14" s="15"/>
-    </row>
-    <row r="15" spans="2:11" ht="40" x14ac:dyDescent="0.2">
-      <c r="B15" s="14" t="s">
+      <c r="H15" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="C15" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="F15" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G15" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="H15" s="30"/>
-      <c r="I15" s="15"/>
-    </row>
-    <row r="16" spans="2:11" ht="61" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F16" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="G16" s="6" t="s">
+      <c r="I15" s="36" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="2"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="17"/>
+    </row>
+    <row r="17" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="H16" s="31" t="s">
-        <v>60</v>
-      </c>
-      <c r="I16" s="18"/>
-    </row>
-    <row r="17" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="2"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="1"/>
-    </row>
-    <row r="18" spans="2:9" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="C18" s="21"/>
-      <c r="D18" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="19" spans="2:9" ht="40" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="20" spans="2:9" ht="40" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="21" spans="2:9" ht="40" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="39" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" ht="40" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" spans="2:4" ht="40" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" spans="2:4" ht="40" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="3">
     <mergeCell ref="B1:I1"/>
-    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B17:C17"/>
     <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>